<commit_message>
predict page -- choose file, prediction table, download file
</commit_message>
<xml_diff>
--- a/source/uploads/first_test_data_credit_default.xlsx
+++ b/source/uploads/first_test_data_credit_default.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="57">
   <si>
     <t>PAY_0</t>
   </si>
@@ -55,139 +55,136 @@
     <t>ID</t>
   </si>
   <si>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>0.82</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>0.63</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.74</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>0.87</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>0.57</t>
+  </si>
+  <si>
+    <t>0.77</t>
+  </si>
+  <si>
     <t>0.88</t>
   </si>
   <si>
-    <t>0.86</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>0.52</t>
-  </si>
-  <si>
-    <t>0.68</t>
-  </si>
-  <si>
-    <t>0.7</t>
-  </si>
-  <si>
-    <t>0.63</t>
-  </si>
-  <si>
-    <t>0.64</t>
-  </si>
-  <si>
-    <t>0.73</t>
-  </si>
-  <si>
-    <t>0.96</t>
-  </si>
-  <si>
-    <t>0.81</t>
-  </si>
-  <si>
     <t>0.78</t>
   </si>
   <si>
-    <t>0.84</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>0.97</t>
-  </si>
-  <si>
-    <t>0.67</t>
-  </si>
-  <si>
-    <t>0.71</t>
-  </si>
-  <si>
-    <t>0.83</t>
-  </si>
-  <si>
-    <t>0.99</t>
-  </si>
-  <si>
-    <t>0.76</t>
-  </si>
-  <si>
-    <t>0.66</t>
-  </si>
-  <si>
-    <t>0.6</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>0.82</t>
-  </si>
-  <si>
-    <t>0.69</t>
-  </si>
-  <si>
-    <t>0.91</t>
-  </si>
-  <si>
-    <t>0.87</t>
-  </si>
-  <si>
     <t>0.65</t>
   </si>
   <si>
-    <t>0.57</t>
-  </si>
-  <si>
     <t>0.94</t>
   </si>
   <si>
-    <t>0.62</t>
-  </si>
-  <si>
-    <t>0.95</t>
-  </si>
-  <si>
     <t>0.55</t>
-  </si>
-  <si>
-    <t>0.51</t>
-  </si>
-  <si>
-    <t>0.77</t>
-  </si>
-  <si>
-    <t>0.59</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>0.85</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.79</t>
-  </si>
-  <si>
-    <t>0.58</t>
-  </si>
-  <si>
-    <t>0.53</t>
-  </si>
-  <si>
-    <t>0.74</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
-    <t>0.5</t>
   </si>
 </sst>
 </file>
@@ -876,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -955,10 +952,10 @@
         <v>432</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -996,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" t="s">
         <v>20</v>
@@ -1040,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1081,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1122,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1163,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="M15" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1204,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1242,10 +1239,10 @@
         <v>1100</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1286,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1327,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1368,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1406,10 +1403,10 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1450,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1491,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1532,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1573,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1611,10 +1608,10 @@
         <v>5398</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1652,10 +1649,10 @@
         <v>1001</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -1696,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1737,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -1775,10 +1772,10 @@
         <v>2044</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1819,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="M31" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1860,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="M32" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1901,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1942,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="M34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -1983,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2024,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2065,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2106,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2147,7 +2144,7 @@
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2188,7 +2185,7 @@
         <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2229,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2311,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="M43" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2352,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="M44" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -2393,7 +2390,7 @@
         <v>0</v>
       </c>
       <c r="M45" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -2431,10 +2428,10 @@
         <v>0</v>
       </c>
       <c r="L46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2516,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="M48" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -2598,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="M50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -2639,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="M51" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -2680,7 +2677,7 @@
         <v>1</v>
       </c>
       <c r="M52" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -2721,7 +2718,7 @@
         <v>0</v>
       </c>
       <c r="M53" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -2762,7 +2759,7 @@
         <v>0</v>
       </c>
       <c r="M54" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -2800,10 +2797,10 @@
         <v>1762</v>
       </c>
       <c r="L55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M55" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -2841,10 +2838,10 @@
         <v>1049</v>
       </c>
       <c r="L56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M56" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -2885,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="M57" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -2926,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="M58" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -2967,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="M59" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -3008,7 +3005,7 @@
         <v>1</v>
       </c>
       <c r="M60" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -3049,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="M61" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -3090,7 +3087,7 @@
         <v>1</v>
       </c>
       <c r="M62" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -3131,7 +3128,7 @@
         <v>0</v>
       </c>
       <c r="M63" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -3172,7 +3169,7 @@
         <v>1</v>
       </c>
       <c r="M64" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -3213,7 +3210,7 @@
         <v>1</v>
       </c>
       <c r="M65" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -3254,7 +3251,7 @@
         <v>1</v>
       </c>
       <c r="M66" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67" spans="1:13">
@@ -3295,7 +3292,7 @@
         <v>1</v>
       </c>
       <c r="M67" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="68" spans="1:13">
@@ -3336,7 +3333,7 @@
         <v>1</v>
       </c>
       <c r="M68" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:13">
@@ -3374,10 +3371,10 @@
         <v>2280</v>
       </c>
       <c r="L69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M69" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -3415,10 +3412,10 @@
         <v>20161</v>
       </c>
       <c r="L70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M70" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -3456,10 +3453,10 @@
         <v>1000</v>
       </c>
       <c r="L71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M71" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:13">
@@ -3500,7 +3497,7 @@
         <v>0</v>
       </c>
       <c r="M72" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:13">
@@ -3541,7 +3538,7 @@
         <v>1</v>
       </c>
       <c r="M73" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:13">
@@ -3582,7 +3579,7 @@
         <v>0</v>
       </c>
       <c r="M74" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:13">
@@ -3620,10 +3617,10 @@
         <v>0</v>
       </c>
       <c r="L75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M75" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="1:13">
@@ -3664,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="M76" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" spans="1:13">
@@ -3705,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="M77" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="78" spans="1:13">
@@ -3746,7 +3743,7 @@
         <v>1</v>
       </c>
       <c r="M78" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -3784,10 +3781,10 @@
         <v>291</v>
       </c>
       <c r="L79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M79" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -3828,7 +3825,7 @@
         <v>1</v>
       </c>
       <c r="M80" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -3869,7 +3866,7 @@
         <v>1</v>
       </c>
       <c r="M81" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -3910,7 +3907,7 @@
         <v>0</v>
       </c>
       <c r="M82" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:13">
@@ -3951,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="M83" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:13">
@@ -3992,7 +3989,7 @@
         <v>1</v>
       </c>
       <c r="M84" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:13">
@@ -4033,7 +4030,7 @@
         <v>0</v>
       </c>
       <c r="M85" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -4074,7 +4071,7 @@
         <v>0</v>
       </c>
       <c r="M86" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:13">
@@ -4115,7 +4112,7 @@
         <v>0</v>
       </c>
       <c r="M87" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="88" spans="1:13">
@@ -4156,7 +4153,7 @@
         <v>1</v>
       </c>
       <c r="M88" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="89" spans="1:13">
@@ -4197,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="M89" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="90" spans="1:13">
@@ -4279,7 +4276,7 @@
         <v>1</v>
       </c>
       <c r="M91" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="1:13">
@@ -4358,10 +4355,10 @@
         <v>0</v>
       </c>
       <c r="L93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M93" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="94" spans="1:13">
@@ -4402,7 +4399,7 @@
         <v>0</v>
       </c>
       <c r="M94" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="95" spans="1:13">
@@ -4443,7 +4440,7 @@
         <v>0</v>
       </c>
       <c r="M95" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="96" spans="1:13">
@@ -4484,7 +4481,7 @@
         <v>1</v>
       </c>
       <c r="M96" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="1:13">
@@ -4525,7 +4522,7 @@
         <v>0</v>
       </c>
       <c r="M97" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="1:13">
@@ -4566,7 +4563,7 @@
         <v>0</v>
       </c>
       <c r="M98" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="99" spans="1:13">
@@ -4607,7 +4604,7 @@
         <v>0</v>
       </c>
       <c r="M99" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="100" spans="1:13">
@@ -4689,7 +4686,7 @@
         <v>1</v>
       </c>
       <c r="M101" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="102" spans="1:13">
@@ -4730,7 +4727,7 @@
         <v>0</v>
       </c>
       <c r="M102" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="103" spans="1:13">
@@ -4771,7 +4768,7 @@
         <v>0</v>
       </c>
       <c r="M103" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -4812,7 +4809,7 @@
         <v>0</v>
       </c>
       <c r="M104" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="105" spans="1:13">
@@ -4853,7 +4850,7 @@
         <v>1</v>
       </c>
       <c r="M105" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="106" spans="1:13">
@@ -4894,7 +4891,7 @@
         <v>1</v>
       </c>
       <c r="M106" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
     </row>
     <row r="107" spans="1:13">
@@ -4935,7 +4932,7 @@
         <v>1</v>
       </c>
       <c r="M107" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:13">
@@ -4976,7 +4973,7 @@
         <v>0</v>
       </c>
       <c r="M108" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
     </row>
     <row r="109" spans="1:13">
@@ -5017,7 +5014,7 @@
         <v>0</v>
       </c>
       <c r="M109" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="110" spans="1:13">
@@ -5055,10 +5052,10 @@
         <v>133657</v>
       </c>
       <c r="L110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M110" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="111" spans="1:13">
@@ -5096,10 +5093,10 @@
         <v>0</v>
       </c>
       <c r="L111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M111" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
result=yes/no, added % symbol in percentage
</commit_message>
<xml_diff>
--- a/source/uploads/first_test_data_credit_default.xlsx
+++ b/source/uploads/first_test_data_credit_default.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="60">
   <si>
     <t>PAY_0</t>
   </si>
@@ -55,136 +55,145 @@
     <t>ID</t>
   </si>
   <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>0.91</t>
-  </si>
-  <si>
-    <t>0.73</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
-    <t>0.71</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
-    <t>0.67</t>
-  </si>
-  <si>
-    <t>0.76</t>
-  </si>
-  <si>
-    <t>0.98</t>
-  </si>
-  <si>
-    <t>0.93</t>
-  </si>
-  <si>
-    <t>0.81</t>
-  </si>
-  <si>
-    <t>0.64</t>
-  </si>
-  <si>
-    <t>0.61</t>
-  </si>
-  <si>
-    <t>0.66</t>
-  </si>
-  <si>
-    <t>0.83</t>
-  </si>
-  <si>
-    <t>0.96</t>
-  </si>
-  <si>
-    <t>0.69</t>
-  </si>
-  <si>
-    <t>0.84</t>
-  </si>
-  <si>
-    <t>0.56</t>
-  </si>
-  <si>
-    <t>0.86</t>
-  </si>
-  <si>
-    <t>0.82</t>
-  </si>
-  <si>
-    <t>0.68</t>
-  </si>
-  <si>
-    <t>0.63</t>
-  </si>
-  <si>
-    <t>0.85</t>
-  </si>
-  <si>
-    <t>0.74</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>0.7</t>
-  </si>
-  <si>
-    <t>0.62</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.97</t>
-  </si>
-  <si>
-    <t>0.51</t>
-  </si>
-  <si>
-    <t>0.58</t>
-  </si>
-  <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>0.99</t>
-  </si>
-  <si>
-    <t>0.52</t>
-  </si>
-  <si>
-    <t>0.87</t>
-  </si>
-  <si>
-    <t>0.53</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
-    <t>0.77</t>
-  </si>
-  <si>
-    <t>0.88</t>
-  </si>
-  <si>
-    <t>0.78</t>
-  </si>
-  <si>
-    <t>0.65</t>
-  </si>
-  <si>
-    <t>0.94</t>
-  </si>
-  <si>
-    <t>0.55</t>
+    <t>92.00%</t>
+  </si>
+  <si>
+    <t>91.00%</t>
+  </si>
+  <si>
+    <t>73.00%</t>
+  </si>
+  <si>
+    <t>54.00%</t>
+  </si>
+  <si>
+    <t>71.00%</t>
+  </si>
+  <si>
+    <t>75.00%</t>
+  </si>
+  <si>
+    <t>67.00%</t>
+  </si>
+  <si>
+    <t>76.00%</t>
+  </si>
+  <si>
+    <t>98.00%</t>
+  </si>
+  <si>
+    <t>93.00%</t>
+  </si>
+  <si>
+    <t>81.00%</t>
+  </si>
+  <si>
+    <t>63.76%</t>
+  </si>
+  <si>
+    <t>60.83%</t>
+  </si>
+  <si>
+    <t>66.00%</t>
+  </si>
+  <si>
+    <t>83.00%</t>
+  </si>
+  <si>
+    <t>96.00%</t>
+  </si>
+  <si>
+    <t>61.00%</t>
+  </si>
+  <si>
+    <t>69.00%</t>
+  </si>
+  <si>
+    <t>84.00%</t>
+  </si>
+  <si>
+    <t>56.00%</t>
+  </si>
+  <si>
+    <t>86.00%</t>
+  </si>
+  <si>
+    <t>82.00%</t>
+  </si>
+  <si>
+    <t>68.00%</t>
+  </si>
+  <si>
+    <t>63.00%</t>
+  </si>
+  <si>
+    <t>85.00%</t>
+  </si>
+  <si>
+    <t>74.00%</t>
+  </si>
+  <si>
+    <t>89.33%</t>
+  </si>
+  <si>
+    <t>70.00%</t>
+  </si>
+  <si>
+    <t>62.00%</t>
+  </si>
+  <si>
+    <t>90.00%</t>
+  </si>
+  <si>
+    <t>97.00%</t>
+  </si>
+  <si>
+    <t>51.00%</t>
+  </si>
+  <si>
+    <t>89.00%</t>
+  </si>
+  <si>
+    <t>58.00%</t>
+  </si>
+  <si>
+    <t>72.00%</t>
+  </si>
+  <si>
+    <t>99.00%</t>
+  </si>
+  <si>
+    <t>51.50%</t>
+  </si>
+  <si>
+    <t>87.00%</t>
+  </si>
+  <si>
+    <t>53.00%</t>
+  </si>
+  <si>
+    <t>57.00%</t>
+  </si>
+  <si>
+    <t>76.80%</t>
+  </si>
+  <si>
+    <t>88.00%</t>
+  </si>
+  <si>
+    <t>78.00%</t>
+  </si>
+  <si>
+    <t>65.00%</t>
+  </si>
+  <si>
+    <t>77.00%</t>
+  </si>
+  <si>
+    <t>94.00%</t>
+  </si>
+  <si>
+    <t>55.00%</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1693,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1734,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -1775,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="M30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1857,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="M32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1898,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1939,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="M34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2021,7 +2030,7 @@
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2062,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="M37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2103,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2144,7 +2153,7 @@
         <v>0</v>
       </c>
       <c r="M39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2185,7 +2194,7 @@
         <v>1</v>
       </c>
       <c r="M40" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2226,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="M41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2267,7 +2276,7 @@
         <v>0</v>
       </c>
       <c r="M42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2308,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="M43" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2431,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="M46" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2472,7 +2481,7 @@
         <v>1</v>
       </c>
       <c r="M47" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2554,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="M49" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -2595,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="M50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -2636,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="M51" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -2677,7 +2686,7 @@
         <v>1</v>
       </c>
       <c r="M52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -2718,7 +2727,7 @@
         <v>0</v>
       </c>
       <c r="M53" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -2759,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="M54" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -2800,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="M55" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -2841,7 +2850,7 @@
         <v>0</v>
       </c>
       <c r="M56" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -2964,7 +2973,7 @@
         <v>0</v>
       </c>
       <c r="M59" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -3005,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="M60" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -3046,7 +3055,7 @@
         <v>0</v>
       </c>
       <c r="M61" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -3087,7 +3096,7 @@
         <v>1</v>
       </c>
       <c r="M62" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -3128,7 +3137,7 @@
         <v>0</v>
       </c>
       <c r="M63" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -3169,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="M64" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -3210,7 +3219,7 @@
         <v>1</v>
       </c>
       <c r="M65" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -3251,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="M66" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:13">
@@ -3292,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="M67" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:13">
@@ -3333,7 +3342,7 @@
         <v>1</v>
       </c>
       <c r="M68" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:13">
@@ -3415,7 +3424,7 @@
         <v>1</v>
       </c>
       <c r="M70" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -3456,7 +3465,7 @@
         <v>1</v>
       </c>
       <c r="M71" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:13">
@@ -3497,7 +3506,7 @@
         <v>0</v>
       </c>
       <c r="M72" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="1:13">
@@ -3620,7 +3629,7 @@
         <v>1</v>
       </c>
       <c r="M75" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:13">
@@ -3661,7 +3670,7 @@
         <v>0</v>
       </c>
       <c r="M76" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="1:13">
@@ -3743,7 +3752,7 @@
         <v>1</v>
       </c>
       <c r="M78" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -3784,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="M79" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -3825,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="M80" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -3866,7 +3875,7 @@
         <v>1</v>
       </c>
       <c r="M81" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -3989,7 +3998,7 @@
         <v>1</v>
       </c>
       <c r="M84" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="85" spans="1:13">
@@ -4030,7 +4039,7 @@
         <v>0</v>
       </c>
       <c r="M85" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -4071,7 +4080,7 @@
         <v>0</v>
       </c>
       <c r="M86" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="87" spans="1:13">
@@ -4112,7 +4121,7 @@
         <v>0</v>
       </c>
       <c r="M87" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="88" spans="1:13">
@@ -4153,7 +4162,7 @@
         <v>1</v>
       </c>
       <c r="M88" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="89" spans="1:13">
@@ -4194,7 +4203,7 @@
         <v>0</v>
       </c>
       <c r="M89" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:13">
@@ -4235,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="M90" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="1:13">
@@ -4276,7 +4285,7 @@
         <v>1</v>
       </c>
       <c r="M91" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="92" spans="1:13">
@@ -4317,7 +4326,7 @@
         <v>1</v>
       </c>
       <c r="M92" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:13">
@@ -4358,7 +4367,7 @@
         <v>1</v>
       </c>
       <c r="M93" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:13">
@@ -4399,7 +4408,7 @@
         <v>0</v>
       </c>
       <c r="M94" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="95" spans="1:13">
@@ -4440,7 +4449,7 @@
         <v>0</v>
       </c>
       <c r="M95" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="96" spans="1:13">
@@ -4481,7 +4490,7 @@
         <v>1</v>
       </c>
       <c r="M96" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:13">
@@ -4522,7 +4531,7 @@
         <v>0</v>
       </c>
       <c r="M97" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="98" spans="1:13">
@@ -4563,7 +4572,7 @@
         <v>0</v>
       </c>
       <c r="M98" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="99" spans="1:13">
@@ -4604,7 +4613,7 @@
         <v>0</v>
       </c>
       <c r="M99" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="100" spans="1:13">
@@ -4645,7 +4654,7 @@
         <v>0</v>
       </c>
       <c r="M100" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:13">
@@ -4686,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="M101" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102" spans="1:13">
@@ -4727,7 +4736,7 @@
         <v>0</v>
       </c>
       <c r="M102" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:13">
@@ -4768,7 +4777,7 @@
         <v>0</v>
       </c>
       <c r="M103" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -4809,7 +4818,7 @@
         <v>0</v>
       </c>
       <c r="M104" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="105" spans="1:13">
@@ -4850,7 +4859,7 @@
         <v>1</v>
       </c>
       <c r="M105" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="106" spans="1:13">
@@ -4891,7 +4900,7 @@
         <v>1</v>
       </c>
       <c r="M106" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="107" spans="1:13">
@@ -4973,7 +4982,7 @@
         <v>0</v>
       </c>
       <c r="M108" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="109" spans="1:13">
@@ -5055,7 +5064,7 @@
         <v>0</v>
       </c>
       <c r="M110" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="111" spans="1:13">
@@ -5096,7 +5105,7 @@
         <v>0</v>
       </c>
       <c r="M111" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>